<commit_message>
First Power BI Commit
</commit_message>
<xml_diff>
--- a/MockUp.xlsx
+++ b/MockUp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vidamx-my.sharepoint.com/personal/alexisalvarez_grupovidanta_com/Documents/UPDATE/Work/Nueva carpeta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexisalvarez\OneDrive - Grupo Vidanta\UPDATE\Work\21. 29Mar19 - Cuadro Vicepresidencia - INPROCESS\VicepresidenciaCuadradoMagico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="8_{6B0E78A7-1D43-4EC6-826B-6C6453127C13}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{61D7FFEB-2335-4CF8-8997-3E82A764D357}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="6_{46D1F7A4-000E-4E77-8E4D-B53321F3D4E7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{26D9260A-BFE6-476D-8A47-BCEC27E56963}"/>
+    <workbookView xWindow="930" yWindow="-110" windowWidth="18380" windowHeight="11020" xr2:uid="{26D9260A-BFE6-476D-8A47-BCEC27E56963}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +190,15 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -309,10 +318,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -323,28 +329,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -663,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2397D163-DA06-42C7-A702-300F8BC66916}">
   <dimension ref="A2:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -687,48 +699,48 @@
     </row>
     <row r="3" spans="2:7" ht="19" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="4" spans="2:7" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="2:7" ht="26" x14ac:dyDescent="0.6">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="F8" s="12" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="F8" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="2"/>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="1">
@@ -736,17 +748,17 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="8" t="str">
+      <c r="B10" s="7" t="str">
         <f>"Total "&amp;B6</f>
         <v>Total Internacional</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>20000</v>
       </c>
       <c r="D10" s="5">
         <v>0.05</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="11" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="1">
@@ -754,117 +766,117 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>-400000</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="F12" s="18" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="F12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="12">
         <v>-1E-4</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B13" s="2"/>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B16" s="8" t="str">
+      <c r="B16" s="7" t="str">
         <f>"Total "&amp;B6</f>
         <v>Total Internacional</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="26" x14ac:dyDescent="0.6">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="9"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20"/>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
       <c r="F20" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B22" s="8" t="str">
+      <c r="B22" s="7" t="str">
         <f>"Total "&amp;B18</f>
         <v>Total Nacional</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>20000</v>
       </c>
       <c r="D22" s="5">
@@ -880,37 +892,37 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B25" s="2"/>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B28" s="8" t="str">
+      <c r="B28" s="7" t="str">
         <f>"Total "&amp;B18</f>
         <v>Total Nacional</v>
       </c>
@@ -918,18 +930,18 @@
       <c r="D28" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="26" x14ac:dyDescent="0.6">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C33" s="1" t="s">
@@ -940,7 +952,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="1"/>
@@ -948,16 +960,16 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>